<commit_message>
added Statisitics Unit Tests
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,16 +473,16 @@
         <v>2007</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>38916</v>
+        <v>55625</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>52973</v>
+        <v>62500</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2196</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -490,118 +490,10 @@
         <v>2008</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43646</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>57596</v>
+        <v>43416</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>17549</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>2009</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>42492</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>56547</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>17709</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>2010</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>43846</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>54481</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>29093</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>2011</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>47451</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>65403</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>36700</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>2012</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>48243</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>64927</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>44153</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>2013</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>51510</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>67367</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>59954</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>2014</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>50658</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>65779</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>66837</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>794</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -615,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -662,7 +554,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>57354</v>
+        <v>51050</v>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
@@ -671,7 +563,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>45.81%</t>
+          <t>71.43%</t>
         </is>
       </c>
     </row>
@@ -682,7 +574,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46291</v>
+        <v>48750</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
@@ -691,147 +583,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>14.15%</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Новосибирск</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>41580</v>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Нижний Новгород</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>2.69%</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Екатеринбург</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>41091</v>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Казань</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>2.66%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Казань</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>37587</v>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>Ростов-на-Дону</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>2.34%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Самара</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>34091</v>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Новосибирск</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>2.02%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Нижний Новгород</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>33637</v>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>Екатеринбург</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>1.43%</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>Ярославль</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>32744</v>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>Воронеж</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>1.4%</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Краснодар</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>32542</v>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>Самара</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>1.33%</t>
+          <t>28.57%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
creating 2 classes statistics (with multiprocessing and classic) with screenshots
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -487,36 +487,36 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43646</v>
+        <v>42492</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>57596</v>
+        <v>56547</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>17549</v>
+        <v>17709</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>354</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>42492</v>
+        <v>43646</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>56547</v>
+        <v>57596</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17709</v>
+        <v>17549</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>278</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5">
@@ -538,36 +538,36 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>47451</v>
+        <v>48243</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>65403</v>
+        <v>64927</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>36700</v>
+        <v>44153</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>728</v>
+        <v>615</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>48243</v>
+        <v>47451</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>64927</v>
+        <v>65403</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44153</v>
+        <v>36700</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>615</v>
+        <v>728</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
multiprocessing v2.0, without manager
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -487,36 +487,36 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>42492</v>
+        <v>43646</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>56547</v>
+        <v>57596</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>17709</v>
+        <v>17549</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>278</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>43646</v>
+        <v>42492</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>57596</v>
+        <v>56547</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17549</v>
+        <v>17709</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>354</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5">
@@ -538,36 +538,36 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>48243</v>
+        <v>47451</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>64927</v>
+        <v>65403</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>44153</v>
+        <v>36700</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>615</v>
+        <v>728</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>47451</v>
+        <v>48243</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>65403</v>
+        <v>64927</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>36700</v>
+        <v>44153</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>728</v>
+        <v>615</v>
       </c>
     </row>
     <row r="8">

</xml_diff>